<commit_message>
Actualizaciones de ultimos archivos
</commit_message>
<xml_diff>
--- a/1 - Gestión de Producción/KPIs.xlsx
+++ b/1 - Gestión de Producción/KPIs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yeison\Documents\APM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yeison\Documents\GitHub\SediaAutomatica\1 - Gestión de Producción\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EDEB2F7-D5FF-4300-8211-B6F5B04538BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FF4DFF-8863-49CB-B7D2-489252185D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{5C7C91DE-BFF6-4FC9-97A8-24A4843CEF5D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C7C91DE-BFF6-4FC9-97A8-24A4843CEF5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Confiabilidad" sheetId="1" r:id="rId1"/>
@@ -231,7 +231,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -527,17 +527,11 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -545,6 +539,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,16 +567,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>606593</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1473368</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>685800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -599,7 +599,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9220200" y="142875"/>
+          <a:off x="0" y="1609725"/>
           <a:ext cx="4969043" cy="1200150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -911,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B1AC48-FB8F-4DD0-A702-89E6D8243F64}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,7 +920,7 @@
     <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
@@ -1120,7 +1120,7 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1188,19 +1188,19 @@
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="31">
+      <c r="B2" s="29">
         <v>0.26129999999999998</v>
       </c>
-      <c r="C2" s="31">
+      <c r="C2" s="29">
         <v>2.3800000000000002E-2</v>
       </c>
-      <c r="D2" s="31">
+      <c r="D2" s="29">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="E2" s="31">
+      <c r="E2" s="29">
         <v>0.68110000000000004</v>
       </c>
-      <c r="F2" s="31">
+      <c r="F2" s="29">
         <v>3.3599999999999998E-2</v>
       </c>
     </row>
@@ -1208,19 +1208,19 @@
       <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="29">
         <v>0.2404</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="29">
         <v>7.2099999999999997E-2</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="29">
         <v>5.8999999999999999E-3</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="29">
         <v>0.68159999999999998</v>
       </c>
-      <c r="F3" s="31">
+      <c r="F3" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1228,19 +1228,19 @@
       <c r="A4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="29">
         <v>0.26960000000000001</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="29">
         <v>2.4500000000000001E-2</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="29">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="29">
         <v>0.68679999999999997</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="29">
         <v>1.8800000000000001E-2</v>
       </c>
     </row>
@@ -1248,19 +1248,19 @@
       <c r="A5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="29">
         <v>0.14729999999999999</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="29">
         <v>4.9099999999999998E-2</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="29">
         <v>0.1212</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="29">
         <v>0.43790000000000001</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="29">
         <v>0.2445</v>
       </c>
     </row>
@@ -1268,19 +1268,19 @@
       <c r="A6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="29">
         <v>0.442</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="29">
         <v>2.46E-2</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="29">
         <v>0.1021</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="29">
         <v>0.43140000000000001</v>
       </c>
-      <c r="F6" s="31">
+      <c r="F6" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1288,19 +1288,19 @@
       <c r="A7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B7" s="29">
         <v>0.14729999999999999</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="29">
         <v>4.9099999999999998E-2</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="29">
         <v>5.8400000000000001E-2</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="29">
         <v>0.68669999999999998</v>
       </c>
-      <c r="F7" s="31">
+      <c r="F7" s="29">
         <v>5.8400000000000001E-2</v>
       </c>
     </row>
@@ -1308,19 +1308,19 @@
       <c r="A8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="31">
+      <c r="B8" s="29">
         <v>0.36530000000000001</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="29">
         <v>2.4500000000000001E-2</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="29">
         <v>7.6300000000000007E-2</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="29">
         <v>0.53390000000000004</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1328,19 +1328,19 @@
       <c r="A9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="31">
+      <c r="B9" s="29">
         <v>0.3664</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="29">
         <v>2.46E-2</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="29">
         <v>7.2800000000000004E-2</v>
       </c>
-      <c r="E9" s="31">
+      <c r="E9" s="29">
         <v>0.53620000000000001</v>
       </c>
-      <c r="F9" s="31">
+      <c r="F9" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1348,19 +1348,19 @@
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="29">
         <v>0.36530000000000001</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="29">
         <v>2.4500000000000001E-2</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="29">
         <v>7.2900000000000006E-2</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="29">
         <v>0.5373</v>
       </c>
-      <c r="F10" s="31">
+      <c r="F10" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1368,19 +1368,19 @@
       <c r="A11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="31">
+      <c r="B11" s="29">
         <v>2.46E-2</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="29">
         <v>4.9200000000000001E-2</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="29">
         <v>5.4600000000000003E-2</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="29">
         <v>0.87160000000000004</v>
       </c>
-      <c r="F11" s="31">
+      <c r="F11" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1388,19 +1388,19 @@
       <c r="A12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="31">
+      <c r="B12" s="29">
         <v>4.8500000000000001E-2</v>
       </c>
-      <c r="C12" s="31">
+      <c r="C12" s="29">
         <v>7.2700000000000001E-2</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="29">
         <v>5.3199999999999997E-2</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E12" s="29">
         <v>0.82569999999999999</v>
       </c>
-      <c r="F12" s="31">
+      <c r="F12" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1408,19 +1408,19 @@
       <c r="A13" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="31">
+      <c r="B13" s="29">
         <v>9.4999999999999998E-3</v>
       </c>
-      <c r="C13" s="31">
+      <c r="C13" s="29">
         <v>4.7500000000000001E-2</v>
       </c>
-      <c r="D13" s="31">
+      <c r="D13" s="29">
         <v>0.1143</v>
       </c>
-      <c r="E13" s="31">
+      <c r="E13" s="29">
         <v>0.82869999999999999</v>
       </c>
-      <c r="F13" s="31">
+      <c r="F13" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1428,19 +1428,19 @@
       <c r="A14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="31">
+      <c r="B14" s="29">
         <v>7.8399999999999997E-2</v>
       </c>
-      <c r="C14" s="31">
+      <c r="C14" s="29">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D14" s="29">
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="E14" s="31">
+      <c r="E14" s="29">
         <v>0.86909999999999998</v>
       </c>
-      <c r="F14" s="31">
+      <c r="F14" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1448,19 +1448,19 @@
       <c r="A15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="31">
+      <c r="B15" s="29">
         <v>0.30890000000000001</v>
       </c>
-      <c r="C15" s="31">
+      <c r="C15" s="29">
         <v>7.2400000000000006E-2</v>
       </c>
-      <c r="D15" s="31">
+      <c r="D15" s="29">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="E15" s="31">
+      <c r="E15" s="29">
         <v>0.56720000000000004</v>
       </c>
-      <c r="F15" s="31">
+      <c r="F15" s="29">
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
@@ -1468,19 +1468,19 @@
       <c r="A16" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="31">
+      <c r="B16" s="29">
         <v>0.14419999999999999</v>
       </c>
-      <c r="C16" s="31">
+      <c r="C16" s="29">
         <v>4.8099999999999997E-2</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D16" s="29">
         <v>7.6E-3</v>
       </c>
-      <c r="E16" s="31">
+      <c r="E16" s="29">
         <v>0.80010000000000003</v>
       </c>
-      <c r="F16" s="31">
+      <c r="F16" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1488,19 +1488,19 @@
       <c r="A17" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="31">
+      <c r="B17" s="29">
         <v>0.28789999999999999</v>
       </c>
-      <c r="C17" s="31">
+      <c r="C17" s="29">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="D17" s="31">
+      <c r="D17" s="29">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="E17" s="31">
+      <c r="E17" s="29">
         <v>0.62539999999999996</v>
       </c>
-      <c r="F17" s="31">
+      <c r="F17" s="29">
         <v>3.8600000000000002E-2</v>
       </c>
     </row>
@@ -1508,19 +1508,19 @@
       <c r="A18" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="31">
+      <c r="B18" s="29">
         <v>0.14369999999999999</v>
       </c>
-      <c r="C18" s="31">
+      <c r="C18" s="29">
         <v>4.7899999999999998E-2</v>
       </c>
-      <c r="D18" s="31">
+      <c r="D18" s="29">
         <v>1.37E-2</v>
       </c>
-      <c r="E18" s="31">
+      <c r="E18" s="29">
         <v>0.79469999999999996</v>
       </c>
-      <c r="F18" s="31">
+      <c r="F18" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1528,19 +1528,19 @@
       <c r="A19" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="31">
+      <c r="B19" s="29">
         <v>0.2873</v>
       </c>
-      <c r="C19" s="31">
+      <c r="C19" s="29">
         <v>9.5799999999999996E-2</v>
       </c>
-      <c r="D19" s="31">
+      <c r="D19" s="29">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="E19" s="31">
+      <c r="E19" s="29">
         <v>0.56130000000000002</v>
       </c>
-      <c r="F19" s="31">
+      <c r="F19" s="29">
         <v>5.5500000000000001E-2</v>
       </c>
     </row>
@@ -1548,19 +1548,19 @@
       <c r="A20" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="31">
+      <c r="B20" s="29">
         <v>0.38229999999999997</v>
       </c>
-      <c r="C20" s="31">
+      <c r="C20" s="29">
         <v>1E-4</v>
       </c>
-      <c r="D20" s="31">
+      <c r="D20" s="29">
         <v>2.2100000000000002E-2</v>
       </c>
-      <c r="E20" s="31">
+      <c r="E20" s="29">
         <v>0.59540000000000004</v>
       </c>
-      <c r="F20" s="31">
+      <c r="F20" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1568,19 +1568,19 @@
       <c r="A21" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="31">
+      <c r="B21" s="29">
         <v>7.1300000000000002E-2</v>
       </c>
-      <c r="C21" s="31">
+      <c r="C21" s="29">
         <v>2.3800000000000002E-2</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D21" s="29">
         <v>1.11E-2</v>
       </c>
-      <c r="E21" s="31">
+      <c r="E21" s="29">
         <v>0.89390000000000003</v>
       </c>
-      <c r="F21" s="31">
+      <c r="F21" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1588,19 +1588,19 @@
       <c r="A22" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="31">
+      <c r="B22" s="29">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="C22" s="31">
+      <c r="C22" s="29">
         <v>0.19189999999999999</v>
       </c>
-      <c r="D22" s="31">
+      <c r="D22" s="29">
         <v>2.41E-2</v>
       </c>
-      <c r="E22" s="31">
+      <c r="E22" s="29">
         <v>0.68810000000000004</v>
       </c>
-      <c r="F22" s="31">
+      <c r="F22" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1608,19 +1608,19 @@
       <c r="A23" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="31">
+      <c r="B23" s="29">
         <v>0.1915</v>
       </c>
-      <c r="C23" s="31">
+      <c r="C23" s="29">
         <v>4.7899999999999998E-2</v>
       </c>
-      <c r="D23" s="31">
+      <c r="D23" s="29">
         <v>0.10680000000000001</v>
       </c>
-      <c r="E23" s="31">
+      <c r="E23" s="29">
         <v>0.65380000000000005</v>
       </c>
-      <c r="F23" s="31">
+      <c r="F23" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1628,19 +1628,19 @@
       <c r="A24" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="31">
+      <c r="B24" s="29">
         <v>0.85160000000000002</v>
       </c>
-      <c r="C24" s="31">
+      <c r="C24" s="29">
         <v>4.7300000000000002E-2</v>
       </c>
-      <c r="D24" s="31">
+      <c r="D24" s="29">
         <v>1E-3</v>
       </c>
-      <c r="E24" s="31">
-        <v>0</v>
-      </c>
-      <c r="F24" s="31">
+      <c r="E24" s="29">
+        <v>0</v>
+      </c>
+      <c r="F24" s="29">
         <v>0.1002</v>
       </c>
     </row>
@@ -1648,19 +1648,19 @@
       <c r="A25" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="31">
+      <c r="B25" s="29">
         <v>7.1499999999999994E-2</v>
       </c>
-      <c r="C25" s="31">
+      <c r="C25" s="29">
         <v>7.1499999999999994E-2</v>
       </c>
-      <c r="D25" s="31">
+      <c r="D25" s="29">
         <v>0.13569999999999999</v>
       </c>
-      <c r="E25" s="31">
+      <c r="E25" s="29">
         <v>0.72119999999999995</v>
       </c>
-      <c r="F25" s="31">
+      <c r="F25" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1668,19 +1668,19 @@
       <c r="A26" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="31">
+      <c r="B26" s="29">
         <v>0.1188</v>
       </c>
-      <c r="C26" s="31">
+      <c r="C26" s="29">
         <v>4.7500000000000001E-2</v>
       </c>
-      <c r="D26" s="31">
+      <c r="D26" s="29">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="E26" s="31">
+      <c r="E26" s="29">
         <v>0.82069999999999999</v>
       </c>
-      <c r="F26" s="31">
+      <c r="F26" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1688,19 +1688,19 @@
       <c r="A27" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="31">
+      <c r="B27" s="29">
         <v>7.0699999999999999E-2</v>
       </c>
-      <c r="C27" s="31">
+      <c r="C27" s="29">
         <v>4.7100000000000003E-2</v>
       </c>
-      <c r="D27" s="31">
+      <c r="D27" s="29">
         <v>0.87919999999999998</v>
       </c>
-      <c r="E27" s="31">
+      <c r="E27" s="29">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="F27" s="31">
+      <c r="F27" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1708,19 +1708,19 @@
       <c r="A28" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="31">
+      <c r="B28" s="29">
         <v>2.3999999999999998E-3</v>
       </c>
-      <c r="C28" s="31">
-        <v>0</v>
-      </c>
-      <c r="D28" s="31">
+      <c r="C28" s="29">
+        <v>0</v>
+      </c>
+      <c r="D28" s="29">
         <v>0.99760000000000004</v>
       </c>
-      <c r="E28" s="31">
-        <v>0</v>
-      </c>
-      <c r="F28" s="31">
+      <c r="E28" s="29">
+        <v>0</v>
+      </c>
+      <c r="F28" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1782,7 +1782,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="32" t="s">
         <v>60</v>
       </c>
       <c r="D33" s="19" t="s">
@@ -1792,21 +1792,21 @@
         <f>B29+C29+D29</f>
         <v>0.37288148148148154</v>
       </c>
-      <c r="F33" s="28">
+      <c r="F33" s="33">
         <f>E33*E34</f>
         <v>0.34390433462367703</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C34" s="26"/>
-      <c r="D34" s="27" t="s">
+      <c r="C34" s="32"/>
+      <c r="D34" s="26" t="s">
         <v>58</v>
       </c>
       <c r="E34" s="24">
         <f>(B29+C29)/(B29+C29+F29)</f>
         <v>0.92228858686498327</v>
       </c>
-      <c r="F34" s="26"/>
+      <c r="F34" s="32"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E35" s="19" t="s">
@@ -1827,17 +1827,17 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="B37" s="30">
+      <c r="B37" s="28">
         <v>0.1</v>
       </c>
       <c r="F37"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="32"/>
-      <c r="B38" s="33"/>
+      <c r="A38" s="30"/>
+      <c r="B38" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1888,19 +1888,19 @@
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="31">
+      <c r="B2" s="29">
         <v>0.48020000000000002</v>
       </c>
-      <c r="C2" s="31">
+      <c r="C2" s="29">
         <v>4.3700000000000003E-2</v>
       </c>
-      <c r="D2" s="31">
+      <c r="D2" s="29">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="E2" s="31">
+      <c r="E2" s="29">
         <v>0.442</v>
       </c>
-      <c r="F2" s="31">
+      <c r="F2" s="29">
         <v>3.3799999999999997E-2</v>
       </c>
     </row>
@@ -1908,19 +1908,19 @@
       <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="29">
         <v>0.42880000000000001</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="29">
         <v>0.12859999999999999</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="29">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="29">
         <v>0.44090000000000001</v>
       </c>
-      <c r="F3" s="31">
+      <c r="F3" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1928,19 +1928,19 @@
       <c r="A4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="29">
         <v>0.47920000000000001</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="29">
         <v>4.36E-2</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="29">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="29">
         <v>0.45639999999999997</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="29">
         <v>2.06E-2</v>
       </c>
     </row>
@@ -1948,19 +1948,19 @@
       <c r="A5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="29">
         <v>0.2515</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="29">
         <v>8.3799999999999999E-2</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="29">
         <v>0.2087</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="29">
         <v>0.20979999999999999</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="29">
         <v>0.24629999999999999</v>
       </c>
     </row>
@@ -1968,19 +1968,19 @@
       <c r="A6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="29">
         <v>0.75380000000000003</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="29">
         <v>4.19E-2</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="29">
         <v>0.18049999999999999</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="29">
         <v>2.3800000000000002E-2</v>
       </c>
-      <c r="F6" s="31">
+      <c r="F6" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1988,19 +1988,19 @@
       <c r="A7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B7" s="29">
         <v>0.2515</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="29">
         <v>8.3799999999999999E-2</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="29">
         <v>0.14099999999999999</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="29">
         <v>0.47049999999999997</v>
       </c>
-      <c r="F7" s="31">
+      <c r="F7" s="29">
         <v>5.33E-2</v>
       </c>
     </row>
@@ -2008,19 +2008,19 @@
       <c r="A8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="31">
+      <c r="B8" s="29">
         <v>0.63080000000000003</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="29">
         <v>4.2299999999999997E-2</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="29">
         <v>0.32690000000000002</v>
       </c>
-      <c r="E8" s="31">
-        <v>0</v>
-      </c>
-      <c r="F8" s="31">
+      <c r="E8" s="29">
+        <v>0</v>
+      </c>
+      <c r="F8" s="29">
         <v>0</v>
       </c>
     </row>
@@ -2028,19 +2028,19 @@
       <c r="A9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="31">
+      <c r="B9" s="29">
         <v>0.62990000000000002</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="29">
         <v>4.2299999999999997E-2</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="29">
         <v>0.32779999999999998</v>
       </c>
-      <c r="E9" s="31">
-        <v>0</v>
-      </c>
-      <c r="F9" s="31">
+      <c r="E9" s="29">
+        <v>0</v>
+      </c>
+      <c r="F9" s="29">
         <v>0</v>
       </c>
     </row>
@@ -2048,19 +2048,19 @@
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="29">
         <v>0.61260000000000003</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="29">
         <v>4.1099999999999998E-2</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="29">
         <v>0.34639999999999999</v>
       </c>
-      <c r="E10" s="31">
-        <v>0</v>
-      </c>
-      <c r="F10" s="31">
+      <c r="E10" s="29">
+        <v>0</v>
+      </c>
+      <c r="F10" s="29">
         <v>0</v>
       </c>
     </row>
@@ -2068,19 +2068,19 @@
       <c r="A11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="31">
+      <c r="B11" s="29">
         <v>4.8800000000000003E-2</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="29">
         <v>9.7500000000000003E-2</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="29">
         <v>0.15260000000000001</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="29">
         <v>0.70109999999999995</v>
       </c>
-      <c r="F11" s="31">
+      <c r="F11" s="29">
         <v>0</v>
       </c>
     </row>
@@ -2088,19 +2088,19 @@
       <c r="A12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="31">
+      <c r="B12" s="29">
         <v>9.0200000000000002E-2</v>
       </c>
-      <c r="C12" s="31">
+      <c r="C12" s="29">
         <v>0.1353</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="29">
         <v>0.1411</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E12" s="29">
         <v>0.63339999999999996</v>
       </c>
-      <c r="F12" s="31">
+      <c r="F12" s="29">
         <v>0</v>
       </c>
     </row>
@@ -2108,19 +2108,19 @@
       <c r="A13" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="31">
+      <c r="B13" s="29">
         <v>1.9400000000000001E-2</v>
       </c>
-      <c r="C13" s="31">
+      <c r="C13" s="29">
         <v>9.7100000000000006E-2</v>
       </c>
-      <c r="D13" s="31">
+      <c r="D13" s="29">
         <v>3.7100000000000001E-2</v>
       </c>
-      <c r="E13" s="31">
+      <c r="E13" s="29">
         <v>0.84640000000000004</v>
       </c>
-      <c r="F13" s="31">
+      <c r="F13" s="29">
         <v>0</v>
       </c>
     </row>
@@ -2128,19 +2128,19 @@
       <c r="A14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="31">
+      <c r="B14" s="29">
         <v>0.1542</v>
       </c>
-      <c r="C14" s="31">
+      <c r="C14" s="29">
         <v>9.6500000000000002E-2</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D14" s="29">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="E14" s="31">
+      <c r="E14" s="29">
         <v>0.70130000000000003</v>
       </c>
-      <c r="F14" s="31">
+      <c r="F14" s="29">
         <v>0</v>
       </c>
     </row>
@@ -2148,19 +2148,19 @@
       <c r="A15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="31">
+      <c r="B15" s="29">
         <v>0.17780000000000001</v>
       </c>
-      <c r="C15" s="31">
+      <c r="C15" s="29">
         <v>8.8900000000000007E-2</v>
       </c>
-      <c r="D15" s="31">
+      <c r="D15" s="29">
         <v>3.0800000000000001E-2</v>
       </c>
-      <c r="E15" s="31">
+      <c r="E15" s="29">
         <v>0.64959999999999996</v>
       </c>
-      <c r="F15" s="31">
+      <c r="F15" s="29">
         <v>5.28E-2</v>
       </c>
     </row>
@@ -2168,19 +2168,19 @@
       <c r="A16" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="31">
+      <c r="B16" s="29">
         <v>0.26190000000000002</v>
       </c>
-      <c r="C16" s="31">
+      <c r="C16" s="29">
         <v>8.7300000000000003E-2</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D16" s="29">
         <v>1.72E-2</v>
       </c>
-      <c r="E16" s="31">
+      <c r="E16" s="29">
         <v>0.63360000000000005</v>
       </c>
-      <c r="F16" s="31">
+      <c r="F16" s="29">
         <v>0</v>
       </c>
     </row>
@@ -2188,19 +2188,19 @@
       <c r="A17" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="31">
+      <c r="B17" s="29">
         <v>0.52010000000000001</v>
       </c>
-      <c r="C17" s="31">
+      <c r="C17" s="29">
         <v>8.6699999999999999E-2</v>
       </c>
-      <c r="D17" s="31">
+      <c r="D17" s="29">
         <v>1E-4</v>
       </c>
-      <c r="E17" s="31">
+      <c r="E17" s="29">
         <v>0.34660000000000002</v>
       </c>
-      <c r="F17" s="31">
+      <c r="F17" s="29">
         <v>4.6399999999999997E-2</v>
       </c>
     </row>
@@ -2208,19 +2208,19 @@
       <c r="A18" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="31">
+      <c r="B18" s="29">
         <v>0.25850000000000001</v>
       </c>
-      <c r="C18" s="31">
+      <c r="C18" s="29">
         <v>8.6199999999999999E-2</v>
       </c>
-      <c r="D18" s="31">
+      <c r="D18" s="29">
         <v>2.4E-2</v>
       </c>
-      <c r="E18" s="31">
+      <c r="E18" s="29">
         <v>0.63129999999999997</v>
       </c>
-      <c r="F18" s="31">
+      <c r="F18" s="29">
         <v>0</v>
       </c>
     </row>
@@ -2228,19 +2228,19 @@
       <c r="A19" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="31">
+      <c r="B19" s="29">
         <v>0.51739999999999997</v>
       </c>
-      <c r="C19" s="31">
+      <c r="C19" s="29">
         <v>0.17249999999999999</v>
       </c>
-      <c r="D19" s="31">
+      <c r="D19" s="29">
         <v>1E-4</v>
       </c>
-      <c r="E19" s="31">
+      <c r="E19" s="29">
         <v>0.25040000000000001</v>
       </c>
-      <c r="F19" s="31">
+      <c r="F19" s="29">
         <v>5.96E-2</v>
       </c>
     </row>
@@ -2248,19 +2248,19 @@
       <c r="A20" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="31">
+      <c r="B20" s="29">
         <v>0.67769999999999997</v>
       </c>
-      <c r="C20" s="31">
+      <c r="C20" s="29">
         <v>1E-4</v>
       </c>
-      <c r="D20" s="31">
+      <c r="D20" s="29">
         <v>1.9E-3</v>
       </c>
-      <c r="E20" s="31">
+      <c r="E20" s="29">
         <v>0.32029999999999997</v>
       </c>
-      <c r="F20" s="31">
+      <c r="F20" s="29">
         <v>0</v>
       </c>
     </row>
@@ -2268,19 +2268,19 @@
       <c r="A21" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="31">
+      <c r="B21" s="29">
         <v>0.14749999999999999</v>
       </c>
-      <c r="C21" s="31">
+      <c r="C21" s="29">
         <v>4.9200000000000001E-2</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D21" s="29">
         <v>0.1527</v>
       </c>
-      <c r="E21" s="31">
+      <c r="E21" s="29">
         <v>0.65069999999999995</v>
       </c>
-      <c r="F21" s="31">
+      <c r="F21" s="29">
         <v>0</v>
       </c>
     </row>
@@ -2288,19 +2288,19 @@
       <c r="A22" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="31">
+      <c r="B22" s="29">
         <v>0.16700000000000001</v>
       </c>
-      <c r="C22" s="31">
+      <c r="C22" s="29">
         <v>0.33429999999999999</v>
       </c>
-      <c r="D22" s="31">
+      <c r="D22" s="29">
         <v>0.49869999999999998</v>
       </c>
-      <c r="E22" s="31">
-        <v>0</v>
-      </c>
-      <c r="F22" s="31">
+      <c r="E22" s="29">
+        <v>0</v>
+      </c>
+      <c r="F22" s="29">
         <v>0</v>
       </c>
     </row>
@@ -2308,19 +2308,19 @@
       <c r="A23" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="31">
+      <c r="B23" s="29">
         <v>0.3337</v>
       </c>
-      <c r="C23" s="31">
+      <c r="C23" s="29">
         <v>8.3599999999999994E-2</v>
       </c>
-      <c r="D23" s="31">
+      <c r="D23" s="29">
         <v>0.58279999999999998</v>
       </c>
-      <c r="E23" s="31">
-        <v>0</v>
-      </c>
-      <c r="F23" s="31">
+      <c r="E23" s="29">
+        <v>0</v>
+      </c>
+      <c r="F23" s="29">
         <v>0</v>
       </c>
     </row>
@@ -2328,19 +2328,19 @@
       <c r="A24" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="31">
+      <c r="B24" s="29">
         <v>0.44700000000000001</v>
       </c>
-      <c r="C24" s="31">
+      <c r="C24" s="29">
         <v>9.3299999999999994E-2</v>
       </c>
-      <c r="D24" s="31">
+      <c r="D24" s="29">
         <v>1E-3</v>
       </c>
-      <c r="E24" s="31">
+      <c r="E24" s="29">
         <v>0.36080000000000001</v>
       </c>
-      <c r="F24" s="31">
+      <c r="F24" s="29">
         <v>9.7900000000000001E-2</v>
       </c>
     </row>
@@ -2348,19 +2348,19 @@
       <c r="A25" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="31">
+      <c r="B25" s="29">
         <v>0.12509999999999999</v>
       </c>
-      <c r="C25" s="31">
+      <c r="C25" s="29">
         <v>0.12509999999999999</v>
       </c>
-      <c r="D25" s="31">
+      <c r="D25" s="29">
         <v>0.74980000000000002</v>
       </c>
-      <c r="E25" s="31">
-        <v>0</v>
-      </c>
-      <c r="F25" s="31">
+      <c r="E25" s="29">
+        <v>0</v>
+      </c>
+      <c r="F25" s="29">
         <v>0</v>
       </c>
     </row>
@@ -2368,19 +2368,19 @@
       <c r="A26" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="31">
+      <c r="B26" s="29">
         <v>0.20849999999999999</v>
       </c>
-      <c r="C26" s="31">
+      <c r="C26" s="29">
         <v>8.3400000000000002E-2</v>
       </c>
-      <c r="D26" s="31">
+      <c r="D26" s="29">
         <v>0.70799999999999996</v>
       </c>
-      <c r="E26" s="31">
-        <v>0</v>
-      </c>
-      <c r="F26" s="31">
+      <c r="E26" s="29">
+        <v>0</v>
+      </c>
+      <c r="F26" s="29">
         <v>0</v>
       </c>
     </row>
@@ -2388,19 +2388,19 @@
       <c r="A27" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="31">
+      <c r="B27" s="29">
         <v>0.13339999999999999</v>
       </c>
-      <c r="C27" s="31">
+      <c r="C27" s="29">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="D27" s="31">
+      <c r="D27" s="29">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="E27" s="31">
+      <c r="E27" s="29">
         <v>0.72799999999999998</v>
       </c>
-      <c r="F27" s="31">
+      <c r="F27" s="29">
         <v>0</v>
       </c>
     </row>
@@ -2408,19 +2408,19 @@
       <c r="A28" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="31">
+      <c r="B28" s="29">
         <v>4.1999999999999997E-3</v>
       </c>
-      <c r="C28" s="31">
-        <v>0</v>
-      </c>
-      <c r="D28" s="31">
+      <c r="C28" s="29">
+        <v>0</v>
+      </c>
+      <c r="D28" s="29">
         <v>0.99580000000000002</v>
       </c>
-      <c r="E28" s="31">
-        <v>0</v>
-      </c>
-      <c r="F28" s="31">
+      <c r="E28" s="29">
+        <v>0</v>
+      </c>
+      <c r="F28" s="29">
         <v>0</v>
       </c>
     </row>
@@ -2481,7 +2481,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="32" t="s">
         <v>60</v>
       </c>
       <c r="D33" s="19" t="s">
@@ -2491,21 +2491,21 @@
         <f>B29+C29+D29</f>
         <v>0.62564814814814818</v>
       </c>
-      <c r="F33" s="28">
+      <c r="F33" s="33">
         <f>E33*E34</f>
         <v>0.59320910038535379</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C34" s="26"/>
-      <c r="D34" s="27" t="s">
+      <c r="C34" s="32"/>
+      <c r="D34" s="26" t="s">
         <v>58</v>
       </c>
       <c r="E34" s="24">
         <f>(B29+C29)/(B29+C29+F29)</f>
         <v>0.94815129260941544</v>
       </c>
-      <c r="F34" s="26"/>
+      <c r="F34" s="32"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E35" s="19" t="s">
@@ -2526,10 +2526,10 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="B37" s="30">
+      <c r="B37" s="28">
         <v>0.02</v>
       </c>
     </row>
@@ -2546,7 +2546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8441A792-CD86-471F-BD02-751B18EC1AC4}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>